<commit_message>
Custom Report updated with suite header
</commit_message>
<xml_diff>
--- a/target/surefire-reports/result-summary.xlsx
+++ b/target/surefire-reports/result-summary.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
-  <si>
-    <t>Suite Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+  <si>
+    <t>Suite Name -TestSuite</t>
   </si>
   <si>
     <t>Class Name</t>
@@ -32,7 +32,16 @@
     <t>Result</t>
   </si>
   <si>
-    <t>TestSuite</t>
+    <t>class com.MavenTest02</t>
+  </si>
+  <si>
+    <t>test01</t>
+  </si>
+  <si>
+    <t>08-Jan-2020 05:25:46</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>class com.MavenTest01</t>
@@ -41,25 +50,10 @@
     <t>testCase2</t>
   </si>
   <si>
-    <t>07-Jan-2020 08:23:42</t>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>08-Jan-2020 05:25:41</t>
   </si>
   <si>
     <t>testCase1</t>
-  </si>
-  <si>
-    <t>07-Jan-2020 08:23:41</t>
-  </si>
-  <si>
-    <t>class com.MavenTest02</t>
-  </si>
-  <si>
-    <t>test01</t>
-  </si>
-  <si>
-    <t>07-Jan-2020 08:23:51</t>
   </si>
 </sst>
 </file>
@@ -81,7 +75,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +120,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -141,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -152,56 +156,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="6">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="B2" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="E2" t="s" s="2">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -212,39 +201,53 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s" s="3">
-        <v>10</v>
+      <c r="C5" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="3">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Logger added and steps of the logs added to html and excel reports
</commit_message>
<xml_diff>
--- a/target/surefire-reports/result-summary.xlsx
+++ b/target/surefire-reports/result-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Suite Name -TestSuite</t>
   </si>
@@ -32,28 +32,84 @@
     <t>Result</t>
   </si>
   <si>
-    <t>class com.MavenTest02</t>
+    <t>Reporter Logs</t>
+  </si>
+  <si>
+    <t>Exception Detail</t>
+  </si>
+  <si>
+    <t>MavenTest01</t>
+  </si>
+  <si>
+    <t>testCase1</t>
+  </si>
+  <si>
+    <t>14-Jan-2020 04:50:09</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MavenTest01.beforeClassStart
+MavenTest01.beforeClassEnd
+MavenTest01.beforeMethodStart
+MavenTest01.beforeMethodEnd
+MavenTest01.testCase1Start
+MavenTest01.testCase1End
+MavenTest01.afterMethodStart
+MavenTest01.afterMethodEnd
+MavenTest01.afterClassStart
+MavenTest01.afterClassEnd
+</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>MavenTest02</t>
   </si>
   <si>
     <t>test01</t>
   </si>
   <si>
-    <t>08-Jan-2020 06:54:17</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>class com.MavenTest01</t>
-  </si>
-  <si>
-    <t>testCase2</t>
-  </si>
-  <si>
-    <t>08-Jan-2020 06:54:11</t>
-  </si>
-  <si>
-    <t>testCase1</t>
+    <t>14-Jan-2020 04:50:14</t>
+  </si>
+  <si>
+    <t>14-Jan-2020 04:50:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MavenTest02.setupStart
+MavenTest02.setupEnd
+MavenTest02.test01Start
+MavenTest02.test01End
+MavenTest02.quitBrowserStart
+MavenTest02.quitBrowserEnd
+</t>
+  </si>
+  <si>
+    <t>MavenTest03</t>
+  </si>
+  <si>
+    <t>14-Jan-2020 04:50:18</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MavenTest03.beforeClassStart
+MavenTest03.beforeClassEnd
+MavenTest03.beforeMethodStart
+MavenTest03.beforeMethodEnd
+MavenTest03.testCase1Start
+MavenTest03.testCase1End
+MavenTest03.afterMethodStart
+MavenTest03.afterMethodEnd
+MavenTest03.afterClassStart
+MavenTest03.afterClassEnd
+</t>
+  </si>
+  <si>
+    <t>expected [false] but found [true]</t>
   </si>
 </sst>
 </file>
@@ -154,7 +210,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -165,11 +223,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="13.2109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.5546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="20.3515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="20.3515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="6.76171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="31.19921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="30.2265625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="6">
@@ -192,61 +259,85 @@
       <c r="E2" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="F2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s" s="3">
+      <c r="F4" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s" s="3">
-        <v>9</v>
+      <c r="C5" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s" s="4">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s" s="4">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>